<commit_message>
Checker werkt, poging tot eigen planning maken
</commit_message>
<xml_diff>
--- a/Timetable.xlsx
+++ b/Timetable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54fb42b29621d9c9/Documents/Project 5 kans 2/GithubCode/Project_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_494107901755860E62355476585DCE3A8746CEC4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECD1A9D2-B460-4433-9DE2-B949336C868D}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_494107901755860E62355476585DCE3A8746CEC4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58810688-C67D-473D-B73D-321FE767CEB7}"/>
   <bookViews>
-    <workbookView xWindow="4164" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -966,6 +966,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1255,7 +1259,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>